<commit_message>
input prep (new exp)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/for paper/input to change.xlsx
+++ b/migforecasting/clustering/for paper/input to change.xlsx
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,1501 +473,3001 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1207.9999999999993</v>
+        <v>2414</v>
       </c>
       <c r="C2" s="2">
-        <v>16635.344249999991</v>
+        <v>19887.443500000001</v>
       </c>
       <c r="D2" s="2">
-        <v>3746.5999999999967</v>
+        <v>8104.9999999999982</v>
       </c>
       <c r="E2" s="2">
-        <v>44.99999999999995</v>
+        <v>473.99999999999983</v>
       </c>
       <c r="F2" s="2">
-        <v>79286.091859999928</v>
+        <v>729883.93608999986</v>
       </c>
       <c r="G2" s="2">
-        <v>30.1</v>
+        <v>39.4</v>
       </c>
       <c r="H2" s="2">
-        <v>32.999999999999773</v>
+        <v>44.999999999999716</v>
       </c>
       <c r="I2" s="2">
-        <v>9.9999999999999485</v>
+        <v>7.99999999999996</v>
       </c>
       <c r="J2" s="2">
-        <v>212.39999999999975</v>
+        <v>296.89999999999964</v>
       </c>
       <c r="K2" s="2">
-        <v>22989.999999999982</v>
+        <v>32143.999999999978</v>
       </c>
       <c r="L2" s="2">
-        <v>7487.889999999994</v>
+        <v>60102.41</v>
       </c>
       <c r="M2" s="2">
-        <v>613356.16829999944</v>
+        <v>550648.19779999938</v>
       </c>
       <c r="N2" s="2">
-        <v>14.999999999999956</v>
+        <v>22.999999999999957</v>
       </c>
       <c r="O2" s="2">
-        <v>672.99999999999989</v>
+        <v>946</v>
       </c>
       <c r="P2" s="2">
-        <v>232900.09079999954</v>
+        <v>236233.54378000001</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>2386</v>
+        <v>10892</v>
       </c>
       <c r="C3" s="2">
-        <v>16273.3732</v>
+        <v>21988.19528</v>
       </c>
       <c r="D3" s="2">
-        <v>10592.199999999999</v>
+        <v>37427.899999999994</v>
       </c>
       <c r="E3" s="2">
-        <v>377.99999999999972</v>
+        <v>807.99999999999966</v>
       </c>
       <c r="F3" s="2">
-        <v>398404.10683999996</v>
+        <v>2824760.7281099996</v>
       </c>
       <c r="G3" s="2">
-        <v>26.4</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2">
-        <v>27.999999999999833</v>
+        <v>78.999999999999503</v>
       </c>
       <c r="I3" s="2">
-        <v>22.999999999999915</v>
+        <v>242.99999999999901</v>
       </c>
       <c r="J3" s="2">
-        <v>800.99999999999955</v>
+        <v>632.49999999999932</v>
       </c>
       <c r="K3" s="2">
-        <v>112136.99999999997</v>
+        <v>959880.00000000023</v>
       </c>
       <c r="L3" s="2">
-        <v>9244.5999999999931</v>
+        <v>322825.61999999994</v>
       </c>
       <c r="M3" s="2">
-        <v>1610842.1835999999</v>
+        <v>12665201.631199995</v>
       </c>
       <c r="N3" s="2">
-        <v>21.999999999999957</v>
+        <v>25.999999999999947</v>
       </c>
       <c r="O3" s="2">
-        <v>624.00000000000011</v>
+        <v>3185</v>
       </c>
       <c r="P3" s="2">
-        <v>1492496.0792400001</v>
+        <v>12405299.012639999</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>6906.9999999999973</v>
+        <v>7235.9999999999973</v>
       </c>
       <c r="C4" s="3">
-        <v>16179.493109999999</v>
+        <v>18166.422620000001</v>
       </c>
       <c r="D4" s="2">
-        <v>45679.399999999994</v>
+        <v>15435.899999999992</v>
       </c>
       <c r="E4" s="2">
-        <v>943.99999999999955</v>
+        <v>2286.9999999999986</v>
       </c>
       <c r="F4" s="2">
-        <v>1135992.2059199996</v>
+        <v>1199846.2190299996</v>
       </c>
       <c r="G4" s="3">
-        <v>22.9</v>
+        <v>30.3</v>
       </c>
       <c r="H4" s="2">
-        <v>86.999999999999389</v>
+        <v>113.99999999999925</v>
       </c>
       <c r="I4" s="2">
-        <v>196.9999999999992</v>
+        <v>57.999999999999737</v>
       </c>
       <c r="J4" s="2">
-        <v>2450.9999999999986</v>
+        <v>664.79999999999927</v>
       </c>
       <c r="K4" s="2">
-        <v>49269.999999999935</v>
+        <v>208310</v>
       </c>
       <c r="L4" s="2">
-        <v>10475.609999999997</v>
+        <v>59763.609999999986</v>
       </c>
       <c r="M4" s="2">
-        <v>832899.14939999871</v>
+        <v>1881565.3498999991</v>
       </c>
       <c r="N4" s="2">
-        <v>26.99999999999994</v>
+        <v>40.999999999999908</v>
       </c>
       <c r="O4" s="2">
-        <v>1959.9999999999998</v>
+        <v>2013.9999999999993</v>
       </c>
       <c r="P4" s="2">
-        <v>1961160.027659998</v>
+        <v>3889344.5399099961</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2">
-        <v>4568.9999999999982</v>
+        <v>3694.0000000000009</v>
       </c>
       <c r="C5" s="2">
-        <v>21418.87329</v>
+        <v>21712.38264</v>
       </c>
       <c r="D5" s="2">
-        <v>4933.5999999999949</v>
+        <v>8165.7999999999993</v>
       </c>
       <c r="E5" s="2">
-        <v>130.99999999999977</v>
+        <v>567.99999999999966</v>
       </c>
       <c r="F5" s="2">
-        <v>143687.26248999985</v>
+        <v>479171.98727999994</v>
       </c>
       <c r="G5" s="2">
-        <v>22.3</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="H5" s="2">
-        <v>103.9999999999993</v>
+        <v>94.999999999999403</v>
       </c>
       <c r="I5" s="2">
-        <v>2.9999999999999765</v>
+        <v>41.999999999999844</v>
       </c>
       <c r="J5" s="2">
-        <v>316.99999999999955</v>
+        <v>556.39999999999964</v>
       </c>
       <c r="K5" s="2">
-        <v>106497.99999999996</v>
+        <v>14808.999999999978</v>
       </c>
       <c r="L5" s="2">
-        <v>19137.909999999989</v>
+        <v>36416.79</v>
       </c>
       <c r="M5" s="2">
-        <v>3427876.6054999977</v>
+        <v>4968189.5378400004</v>
       </c>
       <c r="N5" s="2">
-        <v>50.999999999999886</v>
+        <v>23.99999999999994</v>
       </c>
       <c r="O5" s="2">
-        <v>1217.9999999999995</v>
+        <v>958.99999999999977</v>
       </c>
       <c r="P5" s="2">
-        <v>3524494.8488999987</v>
+        <v>1727129.7467999991</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2">
-        <v>2093.9999999999991</v>
+        <v>4213</v>
       </c>
       <c r="C6" s="2">
-        <v>16955.84604</v>
+        <v>18718.034879999999</v>
       </c>
       <c r="D6" s="2">
-        <v>7192.4999999999927</v>
+        <v>15706.399999999994</v>
       </c>
       <c r="E6" s="2">
-        <v>449.99999999999943</v>
+        <v>1185.9999999999993</v>
       </c>
       <c r="F6" s="2">
-        <v>298227.95619999972</v>
+        <v>912846.19063000008</v>
       </c>
       <c r="G6" s="2">
-        <v>30.03</v>
+        <v>36.5</v>
       </c>
       <c r="H6" s="2">
-        <v>59.999999999999581</v>
+        <v>107.99999999999929</v>
       </c>
       <c r="I6" s="2">
-        <v>14.999999999999922</v>
+        <v>91.999999999999645</v>
       </c>
       <c r="J6" s="2">
-        <v>647.79999999999916</v>
+        <v>873.59999999999934</v>
       </c>
       <c r="K6" s="2">
-        <v>25719.999999999982</v>
+        <v>127582.99999999996</v>
       </c>
       <c r="L6" s="2">
-        <v>20804.14999999998</v>
+        <v>56902.999999999993</v>
       </c>
       <c r="M6" s="2">
-        <v>1533618.0888999989</v>
+        <v>5517088.4192999983</v>
       </c>
       <c r="N6" s="2">
-        <v>21.999999999999932</v>
+        <v>38.999999999999915</v>
       </c>
       <c r="O6" s="2">
-        <v>676.99999999999955</v>
+        <v>1113.0000000000002</v>
       </c>
       <c r="P6" s="2">
-        <v>1868542.2159599983</v>
+        <v>6142682.3205399979</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B7" s="2">
-        <v>2815</v>
+        <v>3948</v>
       </c>
       <c r="C7" s="2">
-        <v>20675.747319999999</v>
+        <v>16306.88399</v>
       </c>
       <c r="D7" s="2">
-        <v>4044.4999999999973</v>
+        <v>11177.6</v>
       </c>
       <c r="E7" s="2">
-        <v>387.99999999999983</v>
+        <v>691.99999999999966</v>
       </c>
       <c r="F7" s="2">
-        <v>509272.59583999997</v>
+        <v>815485.63283999986</v>
       </c>
       <c r="G7" s="2">
-        <v>29.82</v>
+        <v>28.6</v>
       </c>
       <c r="H7" s="2">
-        <v>53.999999999999659</v>
+        <v>96.999999999999389</v>
       </c>
       <c r="I7" s="2">
-        <v>31.999999999999865</v>
+        <v>63.999999999999744</v>
       </c>
       <c r="J7" s="2">
-        <v>1231.9999999999993</v>
+        <v>889.29999999999927</v>
       </c>
       <c r="K7" s="2">
-        <v>47001.999999999993</v>
+        <v>29091.999999999985</v>
       </c>
       <c r="L7" s="2">
-        <v>8969.9999999999982</v>
+        <v>64303.80999999999</v>
       </c>
       <c r="M7" s="2">
-        <v>2998146.3123999988</v>
+        <v>894989.54199999874</v>
       </c>
       <c r="N7" s="2">
-        <v>21.99999999999995</v>
+        <v>31.999999999999918</v>
       </c>
       <c r="O7" s="2">
-        <v>1535</v>
+        <v>1646</v>
       </c>
       <c r="P7" s="2">
-        <v>4597855.1592400009</v>
+        <v>2503429.8272599983</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B8" s="2">
-        <v>2624.9999999999973</v>
+        <v>3246.9999999999968</v>
       </c>
       <c r="C8" s="2">
-        <v>19000.342280000001</v>
+        <v>22498.426080000001</v>
       </c>
       <c r="D8" s="2">
-        <v>12773.499999999993</v>
+        <v>6459.0999999999967</v>
       </c>
       <c r="E8" s="2">
-        <v>480.99999999999943</v>
+        <v>1088.9999999999989</v>
       </c>
       <c r="F8" s="2">
-        <v>477102.61020999961</v>
+        <v>621232.85015999957</v>
       </c>
       <c r="G8" s="2">
-        <v>32.450000000000003</v>
+        <v>29.25</v>
       </c>
       <c r="H8" s="2">
-        <v>83.999999999999417</v>
+        <v>50.999999999999659</v>
       </c>
       <c r="I8" s="2">
-        <v>66.999999999999702</v>
+        <v>23.99999999999989</v>
       </c>
       <c r="J8" s="2">
-        <v>586.09999999999911</v>
+        <v>591.49999999999932</v>
       </c>
       <c r="K8" s="2">
-        <v>13303.999999999976</v>
+        <v>17366.999999999989</v>
       </c>
       <c r="L8" s="2">
-        <v>31991.309999999979</v>
+        <v>79477.839999999967</v>
       </c>
       <c r="M8" s="2">
-        <v>2339528.8654999975</v>
+        <v>2193016.3343999982</v>
       </c>
       <c r="N8" s="2">
-        <v>40.999999999999879</v>
+        <v>29.999999999999911</v>
       </c>
       <c r="O8" s="2">
-        <v>960.99999999999955</v>
+        <v>1564.9999999999991</v>
       </c>
       <c r="P8" s="2">
-        <v>507575.87836999819</v>
+        <v>1421570.0404799981</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B9" s="2">
-        <v>2241.9999999999986</v>
+        <v>2323.9999999999991</v>
       </c>
       <c r="C9" s="2">
-        <v>18928.538</v>
+        <v>15907.71135</v>
       </c>
       <c r="D9" s="2">
-        <v>5624.599999999994</v>
+        <v>7991.9999999999982</v>
       </c>
       <c r="E9" s="2">
-        <v>253.99999999999974</v>
+        <v>39.999999999999901</v>
       </c>
       <c r="F9" s="2">
-        <v>305353.16715999978</v>
+        <v>133791.38202999989</v>
       </c>
       <c r="G9" s="2">
-        <v>28.41</v>
+        <v>31.1</v>
       </c>
       <c r="H9" s="2">
-        <v>54.999999999999609</v>
+        <v>79.999999999999503</v>
       </c>
       <c r="I9" s="2">
-        <v>34.999999999999837</v>
+        <v>22.999999999999893</v>
       </c>
       <c r="J9" s="2">
-        <v>982.89999999999884</v>
+        <v>524.09999999999968</v>
       </c>
       <c r="K9" s="2">
-        <v>22820.999999999982</v>
+        <v>29622.999999999985</v>
       </c>
       <c r="L9" s="2">
-        <v>13234.999999999989</v>
+        <v>43840.999999999985</v>
       </c>
       <c r="M9" s="2">
-        <v>1244565.0463999989</v>
+        <v>1160238.6936999995</v>
       </c>
       <c r="N9" s="2">
-        <v>24.999999999999929</v>
+        <v>22.99999999999994</v>
       </c>
       <c r="O9" s="2">
-        <v>693.99999999999932</v>
+        <v>840</v>
       </c>
       <c r="P9" s="2">
-        <v>3344506.7167999977</v>
+        <v>310629.55309999897</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10" s="2">
-        <v>1255.9999999999986</v>
+        <v>1564.9999999999989</v>
       </c>
       <c r="C10" s="2">
-        <v>16376.46312</v>
+        <v>17400.493439999998</v>
       </c>
       <c r="D10" s="2">
-        <v>6331.8999999999915</v>
+        <v>5934.2999999999947</v>
       </c>
       <c r="E10" s="2">
-        <v>135.99999999999977</v>
+        <v>258.99999999999966</v>
       </c>
       <c r="F10" s="2">
-        <v>158372.48895999984</v>
+        <v>102640.8412799998</v>
       </c>
       <c r="G10" s="2">
-        <v>25.4</v>
+        <v>27.4</v>
       </c>
       <c r="H10" s="2">
-        <v>45.999999999999659</v>
+        <v>47.999999999999673</v>
       </c>
       <c r="I10" s="2">
-        <v>8.9999999999999467</v>
+        <v>20.999999999999893</v>
       </c>
       <c r="J10" s="2">
-        <v>169.29999999999961</v>
+        <v>308.79999999999956</v>
       </c>
       <c r="K10" s="2">
-        <v>61603.99999999992</v>
+        <v>32438.999999999975</v>
       </c>
       <c r="L10" s="2">
-        <v>13867.999999999985</v>
+        <v>34895.129999999976</v>
       </c>
       <c r="M10" s="2">
-        <v>611275.27679999929</v>
+        <v>836820.54719999898</v>
       </c>
       <c r="N10" s="2">
-        <v>31.99999999999989</v>
+        <v>15.999999999999943</v>
       </c>
       <c r="O10" s="2">
-        <v>405.99999999999937</v>
+        <v>529.99999999999966</v>
       </c>
       <c r="P10" s="2">
-        <v>85781.077479999847</v>
+        <v>391012.65215999895</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11" s="2">
-        <v>1293</v>
-      </c>
-      <c r="C11" s="3">
-        <v>16443.209169999991</v>
-      </c>
-      <c r="D11" s="3">
-        <v>4607.6999999999971</v>
-      </c>
-      <c r="E11" s="3">
-        <v>119.99999999999987</v>
-      </c>
-      <c r="F11" s="3">
-        <v>219599.7193099999</v>
-      </c>
-      <c r="G11" s="3">
-        <v>27.9</v>
+        <v>2908.9999999999977</v>
+      </c>
+      <c r="C11" s="2">
+        <v>15931.32554</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10793.899999999996</v>
+      </c>
+      <c r="E11" s="2">
+        <v>268.9999999999996</v>
+      </c>
+      <c r="F11" s="2">
+        <v>416409.6848999997</v>
+      </c>
+      <c r="G11" s="2">
+        <v>24.2</v>
       </c>
       <c r="H11" s="2">
-        <v>20.999999999999858</v>
+        <v>57.999999999999616</v>
       </c>
       <c r="I11" s="2">
-        <v>17.999999999999915</v>
+        <v>74.999999999999673</v>
       </c>
       <c r="J11" s="2">
-        <v>153.79999999999984</v>
+        <v>219.79999999999964</v>
       </c>
       <c r="K11" s="2">
-        <v>16620.999999999989</v>
+        <v>137192.99999999991</v>
       </c>
       <c r="L11" s="2">
-        <v>11932.299999999996</v>
+        <v>146352.99999999994</v>
       </c>
       <c r="M11" s="2">
-        <v>742537.84159999969</v>
+        <v>1813391.6641999981</v>
       </c>
       <c r="N11" s="2">
-        <v>14.999999999999963</v>
+        <v>28.999999999999922</v>
       </c>
       <c r="O11" s="2">
-        <v>440.99999999999977</v>
+        <v>1071.9999999999995</v>
       </c>
       <c r="P11" s="2">
-        <v>123348.75611999938</v>
+        <v>226704.80354999797</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2">
-        <v>788.99999999999841</v>
+        <v>5725</v>
       </c>
       <c r="C12" s="2">
-        <v>19068.8688</v>
+        <v>20773.66617</v>
       </c>
       <c r="D12" s="2">
-        <v>1820.9999999999964</v>
+        <v>26868.199999999993</v>
       </c>
       <c r="E12" s="2">
-        <v>79.999999999999787</v>
+        <v>1111.9999999999993</v>
       </c>
       <c r="F12" s="2">
-        <v>57968.611199999868</v>
+        <v>1674021.9106300003</v>
       </c>
       <c r="G12" s="2">
-        <v>35.799999999999997</v>
+        <v>22.6</v>
       </c>
       <c r="H12" s="2">
-        <v>12.999999999999892</v>
+        <v>72.999999999999545</v>
       </c>
       <c r="I12" s="2">
-        <v>1.9999999999999847</v>
+        <v>113.99999999999952</v>
       </c>
       <c r="J12" s="2">
-        <v>81.399999999999764</v>
+        <v>350.99999999999966</v>
       </c>
       <c r="K12" s="2">
-        <v>32010.999999999935</v>
+        <v>10711.999999999955</v>
       </c>
       <c r="L12" s="2">
-        <v>1244.4599999999969</v>
+        <v>7011.1399999999894</v>
       </c>
       <c r="M12" s="2">
-        <v>838591.639199998</v>
+        <v>49916.868199999284</v>
       </c>
       <c r="N12" s="2">
-        <v>9.9999999999999591</v>
+        <v>1.9999999999999927</v>
       </c>
       <c r="O12" s="2">
-        <v>251.99999999999952</v>
+        <v>1617.9999999999998</v>
       </c>
       <c r="P12" s="2">
-        <v>750105.80711999815</v>
+        <v>5355232.274249997</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" s="2">
-        <v>4126.9999999999991</v>
+        <v>24379.999999999993</v>
       </c>
       <c r="C13" s="2">
-        <v>20441.322639999999</v>
+        <v>19874.44096</v>
       </c>
       <c r="D13" s="2">
-        <v>17070.69999999999</v>
+        <v>207240.69999999998</v>
       </c>
       <c r="E13" s="2">
-        <v>27.999999999999929</v>
+        <v>1859.9999999999984</v>
       </c>
       <c r="F13" s="2">
-        <v>268457.68935999984</v>
+        <v>5926777.3109299988</v>
       </c>
       <c r="G13" s="2">
-        <v>21.79</v>
+        <v>21.6</v>
       </c>
       <c r="H13" s="2">
-        <v>73.999999999999488</v>
+        <v>311.9999999999979</v>
       </c>
       <c r="I13" s="2">
-        <v>69.999999999999687</v>
+        <v>386.99999999999841</v>
       </c>
       <c r="J13" s="2">
-        <v>202.59999999999971</v>
+        <v>962.79999999999893</v>
       </c>
       <c r="K13" s="2">
-        <v>314708.99999999988</v>
+        <v>8125.9999999999918</v>
       </c>
       <c r="L13" s="2">
-        <v>18979.989999999991</v>
+        <v>44861.889999999948</v>
       </c>
       <c r="M13" s="2">
-        <v>3873762.5743999979</v>
+        <v>199155.57099999874</v>
       </c>
       <c r="N13" s="2">
-        <v>28.999999999999932</v>
+        <v>33.999999999999922</v>
       </c>
       <c r="O13" s="2">
-        <v>1107.9999999999998</v>
+        <v>6249</v>
       </c>
       <c r="P13" s="2">
-        <v>3584846.1060399981</v>
+        <v>15178335.903369986</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2">
-        <v>1887.9999999999989</v>
+        <v>4481.9999999999982</v>
       </c>
       <c r="C14" s="2">
-        <v>18376.923200000001</v>
+        <v>37917.462079999998</v>
       </c>
       <c r="D14" s="2">
-        <v>8486.1999999999953</v>
+        <v>14558.999999999989</v>
       </c>
       <c r="E14" s="2">
-        <v>234.99999999999972</v>
+        <v>609.99999999999943</v>
       </c>
       <c r="F14" s="2">
-        <v>341592.53969999967</v>
+        <v>1282627.8831299993</v>
       </c>
       <c r="G14" s="2">
-        <v>26.3</v>
+        <v>29.1</v>
       </c>
       <c r="H14" s="2">
-        <v>155.99999999999895</v>
+        <v>67.999999999999545</v>
       </c>
       <c r="I14" s="2">
-        <v>56.999999999999723</v>
+        <v>114.99999999999949</v>
       </c>
       <c r="J14" s="2">
-        <v>389.39999999999952</v>
+        <v>358.69999999999959</v>
       </c>
       <c r="K14" s="2">
-        <v>182951.9999999998</v>
+        <v>4886.9999999999818</v>
       </c>
       <c r="L14" s="2">
-        <v>19100.999999999978</v>
+        <v>8000.4999999999918</v>
       </c>
       <c r="M14" s="2">
-        <v>2366184.0724999984</v>
+        <v>794969.88139999914</v>
       </c>
       <c r="N14" s="2">
-        <v>24.999999999999932</v>
+        <v>14.999999999999956</v>
       </c>
       <c r="O14" s="2">
-        <v>790.99999999999943</v>
+        <v>1094.9999999999995</v>
       </c>
       <c r="P14" s="2">
-        <v>322435.87408999965</v>
+        <v>5006117.3553799978</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" s="2">
-        <v>20037.999999999996</v>
+        <v>14881</v>
       </c>
       <c r="C15" s="2">
-        <v>25152.816680000011</v>
+        <v>35840.741759999997</v>
       </c>
       <c r="D15" s="2">
-        <v>72911.599999999991</v>
+        <v>52247.999999999993</v>
       </c>
       <c r="E15" s="2">
-        <v>2549.9999999999977</v>
+        <v>2190.9999999999991</v>
       </c>
       <c r="F15" s="2">
-        <v>4713511.9352799999</v>
+        <v>2740590.23832</v>
       </c>
       <c r="G15" s="2">
-        <v>29.9</v>
+        <v>22.8</v>
       </c>
       <c r="H15" s="2">
-        <v>195.99999999999872</v>
+        <v>240.99999999999852</v>
       </c>
       <c r="I15" s="2">
-        <v>248.99999999999895</v>
+        <v>194.99999999999918</v>
       </c>
       <c r="J15" s="2">
-        <v>1123.1999999999985</v>
+        <v>225.39999999999938</v>
       </c>
       <c r="K15" s="2">
-        <v>1264806.9999999993</v>
+        <v>2243.9999999999036</v>
       </c>
       <c r="L15" s="2">
-        <v>104307.92999999998</v>
+        <v>11420.029999999982</v>
       </c>
       <c r="M15" s="2">
-        <v>2214641.3434399972</v>
+        <v>169468.43350463765</v>
       </c>
       <c r="N15" s="2">
-        <v>34.999999999999915</v>
+        <v>5.9999999999999716</v>
       </c>
       <c r="O15" s="2">
-        <v>6308.9999999999991</v>
+        <v>3302</v>
       </c>
       <c r="P15" s="2">
-        <v>26988496.705479994</v>
+        <v>8353078.9401600007</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" s="2">
-        <v>8680.9999999999982</v>
-      </c>
-      <c r="C16" s="2">
-        <v>19397.3076</v>
-      </c>
-      <c r="D16" s="2">
-        <v>32935.899999999994</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1673.9999999999982</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1330729.4930399999</v>
-      </c>
-      <c r="G16" s="2">
-        <v>25.1</v>
+        <v>13019.999999999993</v>
+      </c>
+      <c r="C16" s="3">
+        <v>21164.783759999998</v>
+      </c>
+      <c r="D16" s="3">
+        <v>56657.999999999985</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1856.999999999998</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3773107.8136799997</v>
+      </c>
+      <c r="G16" s="3">
+        <v>28.1</v>
       </c>
       <c r="H16" s="2">
-        <v>158.99999999999895</v>
+        <v>112.99999999999922</v>
       </c>
       <c r="I16" s="2">
-        <v>184.99999999999918</v>
+        <v>371.99999999999841</v>
       </c>
       <c r="J16" s="2">
-        <v>386.19999999999953</v>
+        <v>995.09999999999877</v>
       </c>
       <c r="K16" s="2">
-        <v>810919.99999999977</v>
+        <v>134789</v>
       </c>
       <c r="L16" s="2">
-        <v>182696</v>
+        <v>68742.999999999971</v>
       </c>
       <c r="M16" s="2">
-        <v>5519372.8535999991</v>
+        <v>5197507.5167999975</v>
       </c>
       <c r="N16" s="2">
-        <v>38.999999999999908</v>
+        <v>51.999999999999872</v>
       </c>
       <c r="O16" s="2">
-        <v>2499.9999999999995</v>
+        <v>3298.9999999999995</v>
       </c>
       <c r="P16" s="2">
-        <v>3749387.5015199976</v>
+        <v>11634696.470159991</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" s="2">
-        <v>1278.9999999999998</v>
+        <v>13204.999999999998</v>
       </c>
       <c r="C17" s="2">
-        <v>2585.4999999999986</v>
+        <v>23396.225760000001</v>
       </c>
       <c r="D17" s="2">
-        <v>281.99999999999972</v>
+        <v>83197.2</v>
       </c>
       <c r="E17" s="2">
-        <v>415783.74875999975</v>
+        <v>1948.9999999999984</v>
       </c>
       <c r="F17" s="2">
-        <v>46.954686477696221</v>
+        <v>3114118.2283199993</v>
       </c>
       <c r="G17" s="2">
-        <v>37.299999999999997</v>
+        <v>28.4</v>
       </c>
       <c r="H17" s="2">
-        <v>16.999999999999883</v>
+        <v>180.99999999999883</v>
       </c>
       <c r="I17" s="2">
-        <v>15.999999999999924</v>
+        <v>201.99999999999909</v>
       </c>
       <c r="J17" s="2">
-        <v>410.99999999999943</v>
+        <v>187.19999999999979</v>
       </c>
       <c r="K17" s="2">
-        <v>89147.199999999983</v>
+        <v>770.99999999998715</v>
       </c>
       <c r="L17" s="2">
-        <v>7671.9999999999945</v>
+        <v>8337.9999999999836</v>
       </c>
       <c r="M17" s="2">
-        <v>2684633.8327999976</v>
+        <v>59104.252799998845</v>
       </c>
       <c r="N17" s="2">
-        <v>18.999999999999947</v>
+        <v>22.99999999999994</v>
       </c>
       <c r="O17" s="2">
-        <v>376.99999999999977</v>
+        <v>4264.9999999999991</v>
       </c>
       <c r="P17" s="2">
-        <v>366113.43699999945</v>
+        <v>14759491.671359997</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B18" s="2">
-        <v>2086.9999999999986</v>
-      </c>
-      <c r="C18" s="3">
-        <v>6433.2999999999956</v>
+        <v>7345</v>
+      </c>
+      <c r="C18" s="2">
+        <v>20933.503919999999</v>
       </c>
       <c r="D18" s="2">
-        <v>210.99999999999983</v>
+        <v>33377.19999999999</v>
       </c>
       <c r="E18" s="2">
-        <v>267414.72803999996</v>
+        <v>634.99999999999943</v>
       </c>
       <c r="F18" s="2">
-        <v>14.994657846809471</v>
-      </c>
-      <c r="G18" s="3">
-        <v>32.08</v>
+        <v>2290850.5860000006</v>
+      </c>
+      <c r="G18" s="2">
+        <v>28.3</v>
       </c>
       <c r="H18" s="2">
-        <v>84.999999999999403</v>
+        <v>130.99999999999915</v>
       </c>
       <c r="I18" s="2">
-        <v>54.999999999999737</v>
+        <v>121.9999999999995</v>
       </c>
       <c r="J18" s="2">
-        <v>537.09999999999934</v>
+        <v>211.59999999999974</v>
       </c>
       <c r="K18" s="2">
-        <v>297093.99999999983</v>
+        <v>19513.999999999989</v>
       </c>
       <c r="L18" s="2">
-        <v>16965.999999999989</v>
+        <v>6673</v>
       </c>
       <c r="M18" s="2">
-        <v>2513116.4799999981</v>
+        <v>174197.10959999921</v>
       </c>
       <c r="N18" s="2">
-        <v>39.999999999999886</v>
+        <v>17.999999999999947</v>
       </c>
       <c r="O18" s="2">
-        <v>810.99999999999943</v>
+        <v>1608</v>
       </c>
       <c r="P18" s="2">
-        <v>1568477.3210399991</v>
+        <v>3699859.1983200009</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B19" s="2">
-        <v>2688.9999999999995</v>
+        <v>6628.9999999999982</v>
       </c>
       <c r="C19" s="2">
-        <v>9015.3999999999905</v>
+        <v>19979.241050000001</v>
       </c>
       <c r="D19" s="2">
-        <v>204.99999999999977</v>
+        <v>24799.299999999996</v>
       </c>
       <c r="E19" s="2">
-        <v>229243.99999999988</v>
+        <v>495.99999999999955</v>
       </c>
       <c r="F19" s="2">
-        <v>10.305880237367379</v>
+        <v>1431726.77079</v>
       </c>
       <c r="G19" s="2">
-        <v>21.93</v>
+        <v>23.4</v>
       </c>
       <c r="H19" s="2">
-        <v>70.999999999999531</v>
+        <v>102.99999999999933</v>
       </c>
       <c r="I19" s="2">
-        <v>30.999999999999837</v>
+        <v>154.99999999999937</v>
       </c>
       <c r="J19" s="2">
-        <v>98.599999999999739</v>
+        <v>206.89999999999966</v>
       </c>
       <c r="K19" s="2">
-        <v>279415.99999999988</v>
+        <v>23897.999999999993</v>
       </c>
       <c r="L19" s="2">
-        <v>4925.9999999999973</v>
+        <v>10754.999999999993</v>
       </c>
       <c r="M19" s="2">
-        <v>3402333.9999999972</v>
+        <v>271809.38029999856</v>
       </c>
       <c r="N19" s="2">
-        <v>20.999999999999943</v>
+        <v>10.999999999999966</v>
       </c>
       <c r="O19" s="2">
-        <v>978.9999999999992</v>
+        <v>1573.9999999999998</v>
       </c>
       <c r="P19" s="2">
-        <v>602011.49999999895</v>
+        <v>2329628.0499</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20" s="2">
-        <v>4696.9999999999991</v>
+        <v>4992.9999999999982</v>
       </c>
       <c r="C20" s="2">
-        <v>27639.699999999986</v>
+        <v>16722.441760000002</v>
       </c>
       <c r="D20" s="2">
-        <v>219.99999999999972</v>
+        <v>30655.999999999985</v>
       </c>
       <c r="E20" s="2">
-        <v>794230.03655999957</v>
+        <v>1037.9999999999993</v>
       </c>
       <c r="F20" s="2">
-        <v>22.599949821016981</v>
+        <v>788151.45435999963</v>
       </c>
       <c r="G20" s="2">
-        <v>22.85</v>
+        <v>25.7</v>
       </c>
       <c r="H20" s="2">
-        <v>125.9999999999992</v>
+        <v>113.99999999999925</v>
       </c>
       <c r="I20" s="2">
-        <v>95.999999999999559</v>
+        <v>121.99999999999946</v>
       </c>
       <c r="J20" s="2">
-        <v>536.7999999999995</v>
+        <v>384.19999999999942</v>
       </c>
       <c r="K20" s="2">
-        <v>378688.00000000006</v>
+        <v>25676.999999999949</v>
       </c>
       <c r="L20" s="2">
-        <v>9071.9999999999927</v>
+        <v>13056.299999999997</v>
       </c>
       <c r="M20" s="2">
-        <v>8906174.1647999976</v>
+        <v>416468.51609999931</v>
       </c>
       <c r="N20" s="2">
-        <v>18.999999999999954</v>
+        <v>26.999999999999929</v>
       </c>
       <c r="O20" s="2">
-        <v>1432.9999999999993</v>
+        <v>1999.9999999999995</v>
       </c>
       <c r="P20" s="2">
-        <v>3135363.9667199976</v>
+        <v>3340485.9510699986</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" s="2">
-        <v>5471</v>
+        <v>6711</v>
       </c>
       <c r="C21" s="2">
-        <v>9993.7999999999938</v>
+        <v>16213.878720000001</v>
       </c>
       <c r="D21" s="2">
-        <v>349.99999999999949</v>
+        <v>21373.399999999998</v>
       </c>
       <c r="E21" s="2">
-        <v>135007.86686999991</v>
+        <v>523.99999999999966</v>
       </c>
       <c r="F21" s="2">
-        <v>4.2340797487925723</v>
+        <v>952980.54330999986</v>
       </c>
       <c r="G21" s="2">
-        <v>22.88</v>
+        <v>24.33</v>
       </c>
       <c r="H21" s="2">
-        <v>126.99999999999916</v>
+        <v>50.99999999999968</v>
       </c>
       <c r="I21" s="2">
-        <v>24.999999999999879</v>
+        <v>87.999999999999631</v>
       </c>
       <c r="J21" s="2">
-        <v>357.59999999999962</v>
+        <v>113.89999999999986</v>
       </c>
       <c r="K21" s="2">
-        <v>532404</v>
+        <v>7999.9999999999436</v>
       </c>
       <c r="L21" s="2">
-        <v>27023.969999999979</v>
+        <v>4292.9999999999982</v>
       </c>
       <c r="M21" s="2">
-        <v>9174521.0092999972</v>
+        <v>57192.097399999264</v>
       </c>
       <c r="N21" s="2">
-        <v>29.999999999999922</v>
+        <v>7.9999999999999725</v>
       </c>
       <c r="O21" s="2">
-        <v>2096.9999999999995</v>
+        <v>2061</v>
       </c>
       <c r="P21" s="2">
-        <v>17566777.100189991</v>
+        <v>3033452.7819099985</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B22" s="2">
-        <v>2819.9999999999991</v>
+        <v>1207.9999999999993</v>
       </c>
       <c r="C22" s="2">
-        <v>17545.93204</v>
+        <v>16635.344249999991</v>
       </c>
       <c r="D22" s="2">
-        <v>16399.19999999999</v>
+        <v>3746.5999999999967</v>
       </c>
       <c r="E22" s="2">
-        <v>346.9999999999996</v>
+        <v>44.99999999999995</v>
       </c>
       <c r="F22" s="2">
-        <v>573514.04293999996</v>
+        <v>79286.091859999928</v>
       </c>
       <c r="G22" s="2">
-        <v>28</v>
+        <v>30.1</v>
       </c>
       <c r="H22" s="2">
-        <v>64.999999999999574</v>
+        <v>32.999999999999773</v>
       </c>
       <c r="I22" s="2">
-        <v>59.999999999999716</v>
+        <v>9.9999999999999485</v>
       </c>
       <c r="J22" s="2">
-        <v>382.49999999999949</v>
+        <v>212.39999999999975</v>
       </c>
       <c r="K22" s="2">
-        <v>39639.999999999935</v>
+        <v>22989.999999999982</v>
       </c>
       <c r="L22" s="2">
-        <v>9314.3999999999924</v>
+        <v>7487.889999999994</v>
       </c>
       <c r="M22" s="2">
-        <v>3234408.7671999987</v>
+        <v>613356.16829999944</v>
       </c>
       <c r="N22" s="2">
-        <v>17.99999999999995</v>
+        <v>14.999999999999956</v>
       </c>
       <c r="O22" s="2">
-        <v>744.99999999999955</v>
+        <v>672.99999999999989</v>
       </c>
       <c r="P22" s="2">
-        <v>828015.21829999797</v>
+        <v>232900.09079999954</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B23" s="2">
-        <v>21239.000000000004</v>
+        <v>2386</v>
       </c>
       <c r="C23" s="2">
-        <v>23604.910929999998</v>
+        <v>16273.3732</v>
       </c>
       <c r="D23" s="2">
-        <v>64664.399999999987</v>
+        <v>10592.199999999999</v>
       </c>
       <c r="E23" s="2">
-        <v>2076.9999999999995</v>
+        <v>377.99999999999972</v>
       </c>
       <c r="F23" s="2">
-        <v>4676977.1911800001</v>
+        <v>398404.10683999996</v>
       </c>
       <c r="G23" s="2">
-        <v>30.2</v>
+        <v>26.4</v>
       </c>
       <c r="H23" s="2">
-        <v>300.99999999999807</v>
+        <v>27.999999999999833</v>
       </c>
       <c r="I23" s="2">
-        <v>303.99999999999869</v>
+        <v>22.999999999999915</v>
       </c>
       <c r="J23" s="2">
-        <v>783.79999999999882</v>
+        <v>800.99999999999955</v>
       </c>
       <c r="K23" s="2">
-        <v>202571.00000000003</v>
+        <v>112136.99999999997</v>
       </c>
       <c r="L23" s="2">
-        <v>87368.909999999974</v>
+        <v>9244.5999999999931</v>
       </c>
       <c r="M23" s="2">
-        <v>8408723.8795999978</v>
+        <v>1610842.1835999999</v>
       </c>
       <c r="N23" s="2">
-        <v>34.999999999999901</v>
+        <v>21.999999999999957</v>
       </c>
       <c r="O23" s="2">
-        <v>4502</v>
+        <v>624.00000000000011</v>
       </c>
       <c r="P23" s="2">
-        <v>19397519.885310002</v>
+        <v>1492496.0792400001</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B24" s="2">
-        <v>15028.999999999996</v>
+        <v>6906.9999999999973</v>
       </c>
       <c r="C24" s="2">
-        <v>25869.387780000001</v>
+        <v>16179.493109999999</v>
       </c>
       <c r="D24" s="2">
-        <v>17235.499999999989</v>
+        <v>45679.399999999994</v>
       </c>
       <c r="E24" s="2">
-        <v>1123.9999999999986</v>
+        <v>943.99999999999955</v>
       </c>
       <c r="F24" s="2">
-        <v>866008.93850999954</v>
+        <v>1135992.2059199996</v>
       </c>
       <c r="G24" s="2">
-        <v>23.8</v>
+        <v>22.9</v>
       </c>
       <c r="H24" s="2">
-        <v>124.99999999999919</v>
+        <v>86.999999999999389</v>
       </c>
       <c r="I24" s="2">
-        <v>194.99999999999915</v>
+        <v>196.9999999999992</v>
       </c>
       <c r="J24" s="2">
-        <v>235.39999999999975</v>
+        <v>2450.9999999999986</v>
       </c>
       <c r="K24" s="2">
-        <v>2168.999999999995</v>
+        <v>49269.999999999935</v>
       </c>
       <c r="L24" s="2">
-        <v>22439.059999999987</v>
+        <v>10475.609999999997</v>
       </c>
       <c r="M24" s="2">
-        <v>259751.15039999882</v>
+        <v>832899.14939999871</v>
       </c>
       <c r="N24" s="2">
-        <v>11.999999999999948</v>
+        <v>26.99999999999994</v>
       </c>
       <c r="O24" s="2">
-        <v>3210.9999999999995</v>
+        <v>1959.9999999999998</v>
       </c>
       <c r="P24" s="2">
-        <v>9430951.7147999946</v>
+        <v>1961160.027659998</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B25" s="2">
-        <v>9192</v>
+        <v>4568.9999999999982</v>
       </c>
       <c r="C25" s="2">
-        <v>21205.026720000002</v>
+        <v>21418.87329</v>
       </c>
       <c r="D25" s="2">
-        <v>59994</v>
+        <v>4933.5999999999949</v>
       </c>
       <c r="E25" s="2">
-        <v>1042.9999999999993</v>
+        <v>130.99999999999977</v>
       </c>
       <c r="F25" s="2">
-        <v>1194600.3487199994</v>
+        <v>143687.26248999985</v>
       </c>
       <c r="G25" s="2">
-        <v>24.81</v>
+        <v>22.3</v>
       </c>
       <c r="H25" s="2">
-        <v>140.99999999999912</v>
+        <v>103.9999999999993</v>
       </c>
       <c r="I25" s="2">
-        <v>92.999999999999559</v>
+        <v>2.9999999999999765</v>
       </c>
       <c r="J25" s="2">
-        <v>563.59999999999923</v>
+        <v>316.99999999999955</v>
       </c>
       <c r="K25" s="2">
-        <v>35895.999999999993</v>
+        <v>106497.99999999996</v>
       </c>
       <c r="L25" s="2">
-        <v>57654.419999999991</v>
+        <v>19137.909999999989</v>
       </c>
       <c r="M25" s="2">
-        <v>8271274.1760000018</v>
+        <v>3427876.6054999977</v>
       </c>
       <c r="N25" s="2">
-        <v>36.999999999999908</v>
+        <v>50.999999999999886</v>
       </c>
       <c r="O25" s="2">
-        <v>3089.9999999999995</v>
+        <v>1217.9999999999995</v>
       </c>
       <c r="P25" s="2">
-        <v>7029925.2345599988</v>
+        <v>3524494.8488999987</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B26" s="2">
-        <v>11442</v>
+        <v>2093.9999999999991</v>
       </c>
       <c r="C26" s="2">
-        <v>18218.315640000001</v>
+        <v>16955.84604</v>
       </c>
       <c r="D26" s="2">
-        <v>69421.599999999991</v>
+        <v>7192.4999999999927</v>
       </c>
       <c r="E26" s="2">
-        <v>79.999999999999517</v>
+        <v>449.99999999999943</v>
       </c>
       <c r="F26" s="2">
-        <v>3389505.0556999999</v>
+        <v>298227.95619999972</v>
       </c>
       <c r="G26" s="2">
-        <v>21.85</v>
+        <v>30.03</v>
       </c>
       <c r="H26" s="2">
-        <v>164.99999999999895</v>
+        <v>59.999999999999581</v>
       </c>
       <c r="I26" s="2">
-        <v>248.99999999999898</v>
+        <v>14.999999999999922</v>
       </c>
       <c r="J26" s="2">
-        <v>369.09999999999923</v>
+        <v>647.79999999999916</v>
       </c>
       <c r="K26" s="2">
-        <v>18256.999999999818</v>
+        <v>25719.999999999982</v>
       </c>
       <c r="L26" s="2">
-        <v>57789.999999999949</v>
+        <v>20804.14999999998</v>
       </c>
       <c r="M26" s="2">
-        <v>521260.11459999764</v>
+        <v>1533618.0888999989</v>
       </c>
       <c r="N26" s="2">
-        <v>5.9999999999999627</v>
+        <v>21.999999999999932</v>
       </c>
       <c r="O26" s="2">
-        <v>3403</v>
+        <v>676.99999999999955</v>
       </c>
       <c r="P26" s="2">
-        <v>5939939.1027600002</v>
+        <v>1868542.2159599983</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B27" s="2">
-        <v>2547.9999999999977</v>
+        <v>2815</v>
       </c>
       <c r="C27" s="2">
-        <v>18638.87111</v>
+        <v>20675.747319999999</v>
       </c>
       <c r="D27" s="2">
-        <v>10254.999999999993</v>
+        <v>4044.4999999999973</v>
       </c>
       <c r="E27" s="2">
-        <v>511.99999999999943</v>
+        <v>387.99999999999983</v>
       </c>
       <c r="F27" s="2">
-        <v>451466.86220999988</v>
+        <v>509272.59583999997</v>
       </c>
       <c r="G27" s="2">
-        <v>25</v>
+        <v>29.82</v>
       </c>
       <c r="H27" s="2">
-        <v>83.999999999999432</v>
+        <v>53.999999999999659</v>
       </c>
       <c r="I27" s="2">
-        <v>32.999999999999851</v>
+        <v>31.999999999999865</v>
       </c>
       <c r="J27" s="2">
-        <v>265.79999999999973</v>
+        <v>1231.9999999999993</v>
       </c>
       <c r="K27" s="2">
-        <v>14455.999999999975</v>
+        <v>47001.999999999993</v>
       </c>
       <c r="L27" s="2">
-        <v>35901.049999999996</v>
+        <v>8969.9999999999982</v>
       </c>
       <c r="M27" s="2">
-        <v>1395103.6922999984</v>
+        <v>2998146.3123999988</v>
       </c>
       <c r="N27" s="2">
-        <v>25.999999999999936</v>
+        <v>21.99999999999995</v>
       </c>
       <c r="O27" s="2">
-        <v>919.99999999999955</v>
+        <v>1535</v>
       </c>
       <c r="P27" s="2">
-        <v>932526.86903999816</v>
+        <v>4597855.1592400009</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B28" s="2">
-        <v>2330.9999999999977</v>
+        <v>2624.9999999999973</v>
       </c>
       <c r="C28" s="2">
-        <v>22823.19152</v>
+        <v>19000.342280000001</v>
       </c>
       <c r="D28" s="2">
-        <v>6715.4999999999927</v>
+        <v>12773.499999999993</v>
       </c>
       <c r="E28" s="2">
-        <v>244.99999999999955</v>
+        <v>480.99999999999943</v>
       </c>
       <c r="F28" s="2">
-        <v>235832.72977999973</v>
+        <v>477102.61020999961</v>
       </c>
       <c r="G28" s="2">
-        <v>27.3</v>
+        <v>32.450000000000003</v>
       </c>
       <c r="H28" s="2">
-        <v>76.99999999999946</v>
+        <v>83.999999999999417</v>
       </c>
       <c r="I28" s="2">
-        <v>7.9999999999999538</v>
+        <v>66.999999999999702</v>
       </c>
       <c r="J28" s="2">
-        <v>81.299999999999784</v>
+        <v>586.09999999999911</v>
       </c>
       <c r="K28" s="2">
-        <v>86576.999999999913</v>
+        <v>13303.999999999976</v>
       </c>
       <c r="L28" s="2">
-        <v>15944.749999999989</v>
+        <v>31991.309999999979</v>
       </c>
       <c r="M28" s="2">
-        <v>1820784.7858999991</v>
+        <v>2339528.8654999975</v>
       </c>
       <c r="N28" s="2">
-        <v>15.99999999999995</v>
+        <v>40.999999999999879</v>
       </c>
       <c r="O28" s="2">
-        <v>729.99999999999955</v>
+        <v>960.99999999999955</v>
       </c>
       <c r="P28" s="2">
-        <v>1460779.4436599989</v>
+        <v>507575.87836999819</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B29" s="2">
-        <v>6011.9999999999982</v>
+        <v>2241.9999999999986</v>
       </c>
       <c r="C29" s="2">
-        <v>18611.958289999999</v>
+        <v>18928.538</v>
       </c>
       <c r="D29" s="2">
-        <v>20455.999999999993</v>
+        <v>5624.599999999994</v>
       </c>
       <c r="E29" s="2">
-        <v>645.99999999999943</v>
+        <v>253.99999999999974</v>
       </c>
       <c r="F29" s="2">
-        <v>899043.39099999995</v>
+        <v>305353.16715999978</v>
       </c>
       <c r="G29" s="2">
-        <v>37.19</v>
+        <v>28.41</v>
       </c>
       <c r="H29" s="2">
-        <v>147.99999999999906</v>
+        <v>54.999999999999609</v>
       </c>
       <c r="I29" s="2">
-        <v>40.999999999999794</v>
+        <v>34.999999999999837</v>
       </c>
       <c r="J29" s="2">
-        <v>618.49999999999932</v>
+        <v>982.89999999999884</v>
       </c>
       <c r="K29" s="2">
-        <v>27023.999999999942</v>
+        <v>22820.999999999982</v>
       </c>
       <c r="L29" s="2">
-        <v>26455.999999999993</v>
+        <v>13234.999999999989</v>
       </c>
       <c r="M29" s="2">
-        <v>2652645.5177999986</v>
+        <v>1244565.0463999989</v>
       </c>
       <c r="N29" s="2">
-        <v>18.99999999999995</v>
+        <v>24.999999999999929</v>
       </c>
       <c r="O29" s="2">
-        <v>1149.9999999999995</v>
+        <v>693.99999999999932</v>
       </c>
       <c r="P29" s="2">
-        <v>6067714.9468499981</v>
+        <v>3344506.7167999977</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B30" s="2">
-        <v>3520.9999999999991</v>
+        <v>1255.9999999999986</v>
       </c>
       <c r="C30" s="2">
-        <v>19147.145039999999</v>
+        <v>16376.46312</v>
       </c>
       <c r="D30" s="2">
-        <v>11267.999999999993</v>
+        <v>6331.8999999999915</v>
       </c>
       <c r="E30" s="2">
-        <v>1097.9999999999991</v>
+        <v>135.99999999999977</v>
       </c>
       <c r="F30" s="2">
-        <v>584236.91447999945</v>
+        <v>158372.48895999984</v>
       </c>
       <c r="G30" s="2">
-        <v>51.2</v>
+        <v>25.4</v>
       </c>
       <c r="H30" s="2">
-        <v>122.99999999999919</v>
+        <v>45.999999999999659</v>
       </c>
       <c r="I30" s="2">
-        <v>36.999999999999829</v>
+        <v>8.9999999999999467</v>
       </c>
       <c r="J30" s="2">
-        <v>408.3999999999993</v>
+        <v>169.29999999999961</v>
       </c>
       <c r="K30" s="2">
-        <v>38837.999999999964</v>
+        <v>61603.99999999992</v>
       </c>
       <c r="L30" s="2">
-        <v>26779.999999999989</v>
+        <v>13867.999999999985</v>
       </c>
       <c r="M30" s="2">
-        <v>2725337.6207999978</v>
+        <v>611275.27679999929</v>
       </c>
       <c r="N30" s="2">
-        <v>16.999999999999954</v>
+        <v>31.99999999999989</v>
       </c>
       <c r="O30" s="2">
-        <v>1043.9999999999995</v>
+        <v>405.99999999999937</v>
       </c>
       <c r="P30" s="2">
-        <v>556306.09055999748</v>
+        <v>85781.077479999847</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1293</v>
+      </c>
+      <c r="C31" s="2">
+        <v>16443.209169999991</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4607.6999999999971</v>
+      </c>
+      <c r="E31" s="2">
+        <v>119.99999999999987</v>
+      </c>
+      <c r="F31" s="2">
+        <v>219599.7193099999</v>
+      </c>
+      <c r="G31" s="2">
+        <v>27.9</v>
+      </c>
+      <c r="H31" s="2">
+        <v>20.999999999999858</v>
+      </c>
+      <c r="I31" s="2">
+        <v>17.999999999999915</v>
+      </c>
+      <c r="J31" s="2">
+        <v>153.79999999999984</v>
+      </c>
+      <c r="K31" s="2">
+        <v>16620.999999999989</v>
+      </c>
+      <c r="L31" s="2">
+        <v>11932.299999999996</v>
+      </c>
+      <c r="M31" s="2">
+        <v>742537.84159999969</v>
+      </c>
+      <c r="N31" s="2">
+        <v>14.999999999999963</v>
+      </c>
+      <c r="O31" s="2">
+        <v>440.99999999999977</v>
+      </c>
+      <c r="P31" s="2">
+        <v>123348.75611999938</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>3</v>
+      </c>
+      <c r="B32" s="2">
+        <v>788.99999999999841</v>
+      </c>
+      <c r="C32" s="2">
+        <v>19068.8688</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1820.9999999999964</v>
+      </c>
+      <c r="E32" s="2">
+        <v>79.999999999999787</v>
+      </c>
+      <c r="F32" s="2">
+        <v>57968.611199999868</v>
+      </c>
+      <c r="G32" s="2">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="H32" s="2">
+        <v>12.999999999999892</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1.9999999999999847</v>
+      </c>
+      <c r="J32" s="2">
+        <v>81.399999999999764</v>
+      </c>
+      <c r="K32" s="2">
+        <v>32010.999999999935</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1244.4599999999969</v>
+      </c>
+      <c r="M32" s="2">
+        <v>838591.639199998</v>
+      </c>
+      <c r="N32" s="2">
+        <v>9.9999999999999591</v>
+      </c>
+      <c r="O32" s="2">
+        <v>251.99999999999952</v>
+      </c>
+      <c r="P32" s="2">
+        <v>750105.80711999815</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2">
+        <v>4126.9999999999991</v>
+      </c>
+      <c r="C33" s="3">
+        <v>20441.322639999999</v>
+      </c>
+      <c r="D33" s="2">
+        <v>17070.69999999999</v>
+      </c>
+      <c r="E33" s="2">
+        <v>27.999999999999929</v>
+      </c>
+      <c r="F33" s="2">
+        <v>268457.68935999984</v>
+      </c>
+      <c r="G33" s="3">
+        <v>21.79</v>
+      </c>
+      <c r="H33" s="2">
+        <v>73.999999999999488</v>
+      </c>
+      <c r="I33" s="2">
+        <v>69.999999999999687</v>
+      </c>
+      <c r="J33" s="2">
+        <v>202.59999999999971</v>
+      </c>
+      <c r="K33" s="2">
+        <v>314708.99999999988</v>
+      </c>
+      <c r="L33" s="2">
+        <v>18979.989999999991</v>
+      </c>
+      <c r="M33" s="2">
+        <v>3873762.5743999979</v>
+      </c>
+      <c r="N33" s="2">
+        <v>28.999999999999932</v>
+      </c>
+      <c r="O33" s="2">
+        <v>1107.9999999999998</v>
+      </c>
+      <c r="P33" s="2">
+        <v>3584846.1060399981</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1887.9999999999989</v>
+      </c>
+      <c r="C34" s="2">
+        <v>18376.923200000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>8486.1999999999953</v>
+      </c>
+      <c r="E34" s="2">
+        <v>234.99999999999972</v>
+      </c>
+      <c r="F34" s="2">
+        <v>341592.53969999967</v>
+      </c>
+      <c r="G34" s="2">
+        <v>26.3</v>
+      </c>
+      <c r="H34" s="2">
+        <v>155.99999999999895</v>
+      </c>
+      <c r="I34" s="2">
+        <v>56.999999999999723</v>
+      </c>
+      <c r="J34" s="2">
+        <v>389.39999999999952</v>
+      </c>
+      <c r="K34" s="2">
+        <v>182951.9999999998</v>
+      </c>
+      <c r="L34" s="2">
+        <v>19100.999999999978</v>
+      </c>
+      <c r="M34" s="2">
+        <v>2366184.0724999984</v>
+      </c>
+      <c r="N34" s="2">
+        <v>24.999999999999932</v>
+      </c>
+      <c r="O34" s="2">
+        <v>790.99999999999943</v>
+      </c>
+      <c r="P34" s="2">
+        <v>322435.87408999965</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>3</v>
+      </c>
+      <c r="B35" s="2">
+        <v>20037.999999999996</v>
+      </c>
+      <c r="C35" s="2">
+        <v>25152.816680000011</v>
+      </c>
+      <c r="D35" s="2">
+        <v>72911.599999999991</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2549.9999999999977</v>
+      </c>
+      <c r="F35" s="2">
+        <v>4713511.9352799999</v>
+      </c>
+      <c r="G35" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="H35" s="2">
+        <v>195.99999999999872</v>
+      </c>
+      <c r="I35" s="2">
+        <v>248.99999999999895</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1123.1999999999985</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1264806.9999999993</v>
+      </c>
+      <c r="L35" s="2">
+        <v>104307.92999999998</v>
+      </c>
+      <c r="M35" s="2">
+        <v>2214641.3434399972</v>
+      </c>
+      <c r="N35" s="2">
+        <v>34.999999999999915</v>
+      </c>
+      <c r="O35" s="2">
+        <v>6308.9999999999991</v>
+      </c>
+      <c r="P35" s="2">
+        <v>26988496.705479994</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>3</v>
+      </c>
+      <c r="B36" s="2">
+        <v>8680.9999999999982</v>
+      </c>
+      <c r="C36" s="2">
+        <v>19397.3076</v>
+      </c>
+      <c r="D36" s="2">
+        <v>32935.899999999994</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1673.9999999999982</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1330729.4930399999</v>
+      </c>
+      <c r="G36" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="H36" s="2">
+        <v>158.99999999999895</v>
+      </c>
+      <c r="I36" s="2">
+        <v>184.99999999999918</v>
+      </c>
+      <c r="J36" s="2">
+        <v>386.19999999999953</v>
+      </c>
+      <c r="K36" s="2">
+        <v>810919.99999999977</v>
+      </c>
+      <c r="L36" s="2">
+        <v>182696</v>
+      </c>
+      <c r="M36" s="2">
+        <v>5519372.8535999991</v>
+      </c>
+      <c r="N36" s="2">
+        <v>38.999999999999908</v>
+      </c>
+      <c r="O36" s="2">
+        <v>2499.9999999999995</v>
+      </c>
+      <c r="P36" s="2">
+        <v>3749387.5015199976</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>3</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1278.9999999999998</v>
+      </c>
+      <c r="C37" s="2">
+        <v>19406.97712</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2585.4999999999986</v>
+      </c>
+      <c r="E37" s="2">
+        <v>281.99999999999972</v>
+      </c>
+      <c r="F37" s="2">
+        <v>415783.74875999975</v>
+      </c>
+      <c r="G37" s="2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="H37" s="2">
+        <v>16.999999999999883</v>
+      </c>
+      <c r="I37" s="2">
+        <v>15.999999999999924</v>
+      </c>
+      <c r="J37" s="2">
+        <v>410.99999999999943</v>
+      </c>
+      <c r="K37" s="2">
+        <v>89147.199999999983</v>
+      </c>
+      <c r="L37" s="2">
+        <v>7671.9999999999945</v>
+      </c>
+      <c r="M37" s="2">
+        <v>2684633.8327999976</v>
+      </c>
+      <c r="N37" s="2">
+        <v>18.999999999999947</v>
+      </c>
+      <c r="O37" s="2">
+        <v>376.99999999999977</v>
+      </c>
+      <c r="P37" s="2">
+        <v>366113.43699999945</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>3</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2086.9999999999986</v>
+      </c>
+      <c r="C38" s="2">
+        <v>17100.190320000002</v>
+      </c>
+      <c r="D38" s="2">
+        <v>6433.2999999999956</v>
+      </c>
+      <c r="E38" s="2">
+        <v>210.99999999999983</v>
+      </c>
+      <c r="F38" s="2">
+        <v>267414.72803999996</v>
+      </c>
+      <c r="G38" s="2">
+        <v>32.08</v>
+      </c>
+      <c r="H38" s="2">
+        <v>84.999999999999403</v>
+      </c>
+      <c r="I38" s="2">
+        <v>54.999999999999737</v>
+      </c>
+      <c r="J38" s="2">
+        <v>537.09999999999934</v>
+      </c>
+      <c r="K38" s="2">
+        <v>297093.99999999983</v>
+      </c>
+      <c r="L38" s="2">
+        <v>16965.999999999989</v>
+      </c>
+      <c r="M38" s="2">
+        <v>2513116.4799999981</v>
+      </c>
+      <c r="N38" s="2">
+        <v>39.999999999999886</v>
+      </c>
+      <c r="O38" s="2">
+        <v>810.99999999999943</v>
+      </c>
+      <c r="P38" s="2">
+        <v>1568477.3210399991</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>3</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2688.9999999999995</v>
+      </c>
+      <c r="C39" s="2">
+        <v>18039.2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>9015.3999999999905</v>
+      </c>
+      <c r="E39" s="2">
+        <v>204.99999999999977</v>
+      </c>
+      <c r="F39" s="2">
+        <v>229243.99999999988</v>
+      </c>
+      <c r="G39" s="2">
+        <v>21.93</v>
+      </c>
+      <c r="H39" s="2">
+        <v>70.999999999999531</v>
+      </c>
+      <c r="I39" s="2">
+        <v>30.999999999999837</v>
+      </c>
+      <c r="J39" s="2">
+        <v>98.599999999999739</v>
+      </c>
+      <c r="K39" s="2">
+        <v>279415.99999999988</v>
+      </c>
+      <c r="L39" s="2">
+        <v>4925.9999999999973</v>
+      </c>
+      <c r="M39" s="2">
+        <v>3402333.9999999972</v>
+      </c>
+      <c r="N39" s="2">
+        <v>20.999999999999943</v>
+      </c>
+      <c r="O39" s="2">
+        <v>978.9999999999992</v>
+      </c>
+      <c r="P39" s="2">
+        <v>602011.49999999895</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>3</v>
+      </c>
+      <c r="B40" s="2">
+        <v>4696.9999999999991</v>
+      </c>
+      <c r="C40" s="2">
+        <v>19598.053680000001</v>
+      </c>
+      <c r="D40" s="2">
+        <v>27639.699999999986</v>
+      </c>
+      <c r="E40" s="2">
+        <v>219.99999999999972</v>
+      </c>
+      <c r="F40" s="2">
+        <v>794230.03655999957</v>
+      </c>
+      <c r="G40" s="2">
+        <v>22.85</v>
+      </c>
+      <c r="H40" s="2">
+        <v>125.9999999999992</v>
+      </c>
+      <c r="I40" s="2">
+        <v>95.999999999999559</v>
+      </c>
+      <c r="J40" s="2">
+        <v>536.7999999999995</v>
+      </c>
+      <c r="K40" s="2">
+        <v>378688.00000000006</v>
+      </c>
+      <c r="L40" s="2">
+        <v>9071.9999999999927</v>
+      </c>
+      <c r="M40" s="2">
+        <v>8906174.1647999976</v>
+      </c>
+      <c r="N40" s="2">
+        <v>18.999999999999954</v>
+      </c>
+      <c r="O40" s="2">
+        <v>1432.9999999999993</v>
+      </c>
+      <c r="P40" s="2">
+        <v>3135363.9667199976</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>3</v>
+      </c>
+      <c r="B41" s="2">
+        <v>5471</v>
+      </c>
+      <c r="C41" s="2">
+        <v>24531.17148999999</v>
+      </c>
+      <c r="D41" s="2">
+        <v>9993.7999999999938</v>
+      </c>
+      <c r="E41" s="2">
+        <v>349.99999999999949</v>
+      </c>
+      <c r="F41" s="2">
+        <v>135007.86686999991</v>
+      </c>
+      <c r="G41" s="2">
+        <v>22.88</v>
+      </c>
+      <c r="H41" s="2">
+        <v>126.99999999999916</v>
+      </c>
+      <c r="I41" s="2">
+        <v>24.999999999999879</v>
+      </c>
+      <c r="J41" s="2">
+        <v>357.59999999999962</v>
+      </c>
+      <c r="K41" s="2">
+        <v>532404</v>
+      </c>
+      <c r="L41" s="2">
+        <v>27023.969999999979</v>
+      </c>
+      <c r="M41" s="2">
+        <v>9174521.0092999972</v>
+      </c>
+      <c r="N41" s="2">
+        <v>29.999999999999922</v>
+      </c>
+      <c r="O41" s="2">
+        <v>2096.9999999999995</v>
+      </c>
+      <c r="P41" s="2">
+        <v>17566777.100189991</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2">
+        <v>11633.999999999998</v>
+      </c>
+      <c r="C42" s="2">
+        <v>24954.799999999999</v>
+      </c>
+      <c r="D42" s="2">
+        <v>37654.999999999985</v>
+      </c>
+      <c r="E42" s="2">
+        <v>898.99999999999943</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1350652</v>
+      </c>
+      <c r="G42" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="H42" s="2">
+        <v>69.999999999999503</v>
+      </c>
+      <c r="I42" s="2">
+        <v>171.99999999999929</v>
+      </c>
+      <c r="J42" s="2">
+        <v>201.0999999999998</v>
+      </c>
+      <c r="K42" s="2">
+        <v>14598.999999999955</v>
+      </c>
+      <c r="L42" s="2">
+        <v>16640.329999999991</v>
+      </c>
+      <c r="M42" s="2">
+        <v>232538.99999999936</v>
+      </c>
+      <c r="N42" s="2">
+        <v>10.999999999999968</v>
+      </c>
+      <c r="O42" s="2">
+        <v>2737.9999999999991</v>
+      </c>
+      <c r="P42" s="2">
+        <v>32418265.199999992</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>4</v>
+      </c>
+      <c r="B43" s="2">
+        <v>6935.9999999999991</v>
+      </c>
+      <c r="C43" s="2">
+        <v>34591.617420000002</v>
+      </c>
+      <c r="D43" s="2">
+        <v>13338.599999999997</v>
+      </c>
+      <c r="E43" s="2">
+        <v>494.99999999999943</v>
+      </c>
+      <c r="F43" s="2">
+        <v>139069.51849999998</v>
+      </c>
+      <c r="G43" s="2">
+        <v>22.9</v>
+      </c>
+      <c r="H43" s="2">
+        <v>76.999999999999531</v>
+      </c>
+      <c r="I43" s="2">
+        <v>124.99999999999952</v>
+      </c>
+      <c r="J43" s="2">
+        <v>169.2999999999999</v>
+      </c>
+      <c r="K43" s="2">
+        <v>19625.999999999978</v>
+      </c>
+      <c r="L43" s="2">
+        <v>10308.619999999997</v>
+      </c>
+      <c r="M43" s="2">
+        <v>429026.07919999963</v>
+      </c>
+      <c r="N43" s="2">
+        <v>11.999999999999972</v>
+      </c>
+      <c r="O43" s="2">
+        <v>2062</v>
+      </c>
+      <c r="P43" s="2">
+        <v>13315114.298400002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>4</v>
+      </c>
+      <c r="B44" s="2">
+        <v>16843</v>
+      </c>
+      <c r="C44" s="2">
+        <v>35339.908029999999</v>
+      </c>
+      <c r="D44" s="2">
+        <v>73491.599999999991</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2645.9999999999991</v>
+      </c>
+      <c r="F44" s="2">
+        <v>2006637.54357</v>
+      </c>
+      <c r="G44" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="H44" s="2">
+        <v>164.99999999999895</v>
+      </c>
+      <c r="I44" s="2">
+        <v>232.99999999999903</v>
+      </c>
+      <c r="J44" s="2">
+        <v>188.49999999999935</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1592.9999999998829</v>
+      </c>
+      <c r="L44" s="2">
+        <v>23405.999999999971</v>
+      </c>
+      <c r="M44" s="2">
+        <v>313421.54109999974</v>
+      </c>
+      <c r="N44" s="2">
+        <v>7.9999999999999671</v>
+      </c>
+      <c r="O44" s="2">
+        <v>5536</v>
+      </c>
+      <c r="P44" s="2">
+        <v>37484508.028549999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2">
+        <v>11292</v>
+      </c>
+      <c r="C45" s="2">
+        <v>23845.612519999999</v>
+      </c>
+      <c r="D45" s="2">
+        <v>33352.599999999984</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1263.9999999999993</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1716389.6294400003</v>
+      </c>
+      <c r="G45" s="2">
+        <v>29.41</v>
+      </c>
+      <c r="H45" s="2">
+        <v>70.999999999999531</v>
+      </c>
+      <c r="I45" s="2">
+        <v>230.99999999999903</v>
+      </c>
+      <c r="J45" s="2">
+        <v>233.29999999999964</v>
+      </c>
+      <c r="K45" s="2">
+        <v>383.99999999993003</v>
+      </c>
+      <c r="L45" s="2">
+        <v>37867.999999999993</v>
+      </c>
+      <c r="M45" s="2">
+        <v>322803.30879999872</v>
+      </c>
+      <c r="N45" s="2">
+        <v>0.99999999999999423</v>
+      </c>
+      <c r="O45" s="2">
+        <v>2426.9999999999995</v>
+      </c>
+      <c r="P45" s="2">
+        <v>32139963.465120006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>4</v>
+      </c>
+      <c r="B46" s="2">
+        <v>33537</v>
+      </c>
+      <c r="C46" s="2">
+        <v>27126.22694</v>
+      </c>
+      <c r="D46" s="2">
+        <v>58200</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2876.9999999999973</v>
+      </c>
+      <c r="F46" s="2">
+        <v>10541809.012150001</v>
+      </c>
+      <c r="G46" s="2">
+        <v>31.4</v>
+      </c>
+      <c r="H46" s="2">
+        <v>306.99999999999795</v>
+      </c>
+      <c r="I46" s="2">
+        <v>198.99999999999918</v>
+      </c>
+      <c r="J46" s="2">
+        <v>474.69999999999879</v>
+      </c>
+      <c r="K46" s="2">
+        <v>595570.99999999977</v>
+      </c>
+      <c r="L46" s="2">
+        <v>59771.349999999991</v>
+      </c>
+      <c r="M46" s="2">
+        <v>1632754.1328999992</v>
+      </c>
+      <c r="N46" s="2">
+        <v>90.999999999999801</v>
+      </c>
+      <c r="O46" s="2">
+        <v>9371</v>
+      </c>
+      <c r="P46" s="2">
+        <v>79424596.731749997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2">
+        <v>18176.000000000004</v>
+      </c>
+      <c r="C47" s="2">
+        <v>23163.327300000001</v>
+      </c>
+      <c r="D47" s="2">
+        <v>31730.199999999993</v>
+      </c>
+      <c r="E47" s="2">
+        <v>917.9999999999992</v>
+      </c>
+      <c r="F47" s="2">
+        <v>452989.22927999997</v>
+      </c>
+      <c r="G47" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="H47" s="2">
+        <v>95.999999999999417</v>
+      </c>
+      <c r="I47" s="2">
+        <v>288.99999999999881</v>
+      </c>
+      <c r="J47" s="2">
+        <v>587.09999999999934</v>
+      </c>
+      <c r="K47" s="2">
+        <v>126725.99999999991</v>
+      </c>
+      <c r="L47" s="2">
+        <v>185639.8</v>
+      </c>
+      <c r="M47" s="2">
+        <v>14552482.084499996</v>
+      </c>
+      <c r="N47" s="2">
+        <v>24.99999999999995</v>
+      </c>
+      <c r="O47" s="2">
+        <v>2873</v>
+      </c>
+      <c r="P47" s="2">
+        <v>36429440.007749997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>4</v>
+      </c>
+      <c r="B48" s="2">
+        <v>7325.9999999999973</v>
+      </c>
+      <c r="C48" s="2">
+        <v>26937.748680000001</v>
+      </c>
+      <c r="D48" s="2">
+        <v>34428.699999999997</v>
+      </c>
+      <c r="E48" s="2">
+        <v>295.99999999999977</v>
+      </c>
+      <c r="F48" s="2">
+        <v>874914.97008999961</v>
+      </c>
+      <c r="G48" s="2">
+        <v>27.8</v>
+      </c>
+      <c r="H48" s="2">
+        <v>71.999999999999531</v>
+      </c>
+      <c r="I48" s="2">
+        <v>61.99999999999973</v>
+      </c>
+      <c r="J48" s="2">
+        <v>326.69999999999953</v>
+      </c>
+      <c r="K48" s="2">
+        <v>242107.99999999991</v>
+      </c>
+      <c r="L48" s="2">
+        <v>22680.459999999981</v>
+      </c>
+      <c r="M48" s="2">
+        <v>1912868.0863999992</v>
+      </c>
+      <c r="N48" s="2">
+        <v>33.999999999999929</v>
+      </c>
+      <c r="O48" s="2">
+        <v>2005.9999999999991</v>
+      </c>
+      <c r="P48" s="2">
+        <v>10106972.212469997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>4</v>
+      </c>
+      <c r="B49" s="2">
+        <v>8685.9999999999982</v>
+      </c>
+      <c r="C49" s="2">
+        <v>42094.553160000003</v>
+      </c>
+      <c r="D49" s="2">
+        <v>24708.299999999988</v>
+      </c>
+      <c r="E49" s="2">
+        <v>784.99999999999943</v>
+      </c>
+      <c r="F49" s="2">
+        <v>235916.11684999964</v>
+      </c>
+      <c r="G49" s="2">
+        <v>24.1</v>
+      </c>
+      <c r="H49" s="2">
+        <v>95.999999999999361</v>
+      </c>
+      <c r="I49" s="2">
+        <v>89.999999999999616</v>
+      </c>
+      <c r="J49" s="2">
+        <v>203.39999999999958</v>
+      </c>
+      <c r="K49" s="2">
+        <v>5408.9999999999827</v>
+      </c>
+      <c r="L49" s="2">
+        <v>10979.999999999987</v>
+      </c>
+      <c r="M49" s="2">
+        <v>284662.70919999992</v>
+      </c>
+      <c r="N49" s="2">
+        <v>22.999999999999936</v>
+      </c>
+      <c r="O49" s="2">
+        <v>2374.9999999999995</v>
+      </c>
+      <c r="P49" s="2">
+        <v>19503601.519479997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>4</v>
+      </c>
+      <c r="B50" s="2">
+        <v>7612.9999999999955</v>
+      </c>
+      <c r="C50" s="2">
+        <v>46334.301520000001</v>
+      </c>
+      <c r="D50" s="2">
+        <v>16250.099999999991</v>
+      </c>
+      <c r="E50" s="2">
+        <v>234.99999999999969</v>
+      </c>
+      <c r="F50" s="2">
+        <v>32648.816119999738</v>
+      </c>
+      <c r="G50" s="2">
+        <v>30</v>
+      </c>
+      <c r="H50" s="2">
+        <v>79.999999999999446</v>
+      </c>
+      <c r="I50" s="2">
+        <v>107.9999999999995</v>
+      </c>
+      <c r="J50" s="2">
+        <v>427.19999999999948</v>
+      </c>
+      <c r="K50" s="2">
+        <v>4131.9999999999918</v>
+      </c>
+      <c r="L50" s="2">
+        <v>8392.9999999999873</v>
+      </c>
+      <c r="M50" s="2">
+        <v>188124.7558999997</v>
+      </c>
+      <c r="N50" s="2">
+        <v>17.99999999999995</v>
+      </c>
+      <c r="O50" s="2">
+        <v>2056.9999999999991</v>
+      </c>
+      <c r="P50" s="2">
+        <v>14058344.947639994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>4</v>
+      </c>
+      <c r="B51" s="2">
+        <v>4205.9999999999991</v>
+      </c>
+      <c r="C51" s="2">
+        <v>19389.94642</v>
+      </c>
+      <c r="D51" s="2">
+        <v>11099.749999999991</v>
+      </c>
+      <c r="E51" s="2">
+        <v>433.9999999999996</v>
+      </c>
+      <c r="F51" s="2">
+        <v>788066.8027999996</v>
+      </c>
+      <c r="G51" s="2">
+        <v>24.92</v>
+      </c>
+      <c r="H51" s="2">
+        <v>97.999999999999346</v>
+      </c>
+      <c r="I51" s="2">
+        <v>39.999999999999808</v>
+      </c>
+      <c r="J51" s="2">
+        <v>809.89999999999918</v>
+      </c>
+      <c r="K51" s="2">
+        <v>34895.999999999935</v>
+      </c>
+      <c r="L51" s="2">
+        <v>20614.999999999989</v>
+      </c>
+      <c r="M51" s="2">
+        <v>3207835.7308999989</v>
+      </c>
+      <c r="N51" s="2">
+        <v>23.999999999999936</v>
+      </c>
+      <c r="O51" s="2">
+        <v>862.99999999999943</v>
+      </c>
+      <c r="P51" s="2">
+        <v>14660212.994809996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>5</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B52" s="2">
+        <v>2819.9999999999991</v>
+      </c>
+      <c r="C52" s="2">
+        <v>17545.93204</v>
+      </c>
+      <c r="D52" s="2">
+        <v>16399.19999999999</v>
+      </c>
+      <c r="E52" s="2">
+        <v>346.9999999999996</v>
+      </c>
+      <c r="F52" s="2">
+        <v>573514.04293999996</v>
+      </c>
+      <c r="G52" s="2">
+        <v>28</v>
+      </c>
+      <c r="H52" s="2">
+        <v>64.999999999999574</v>
+      </c>
+      <c r="I52" s="2">
+        <v>59.999999999999716</v>
+      </c>
+      <c r="J52" s="2">
+        <v>382.49999999999949</v>
+      </c>
+      <c r="K52" s="2">
+        <v>39639.999999999935</v>
+      </c>
+      <c r="L52" s="2">
+        <v>9314.3999999999924</v>
+      </c>
+      <c r="M52" s="2">
+        <v>3234408.7671999987</v>
+      </c>
+      <c r="N52" s="2">
+        <v>17.99999999999995</v>
+      </c>
+      <c r="O52" s="2">
+        <v>744.99999999999955</v>
+      </c>
+      <c r="P52" s="2">
+        <v>828015.21829999797</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>5</v>
+      </c>
+      <c r="B53" s="2">
+        <v>21239.000000000004</v>
+      </c>
+      <c r="C53" s="2">
+        <v>23604.910929999998</v>
+      </c>
+      <c r="D53" s="2">
+        <v>64664.399999999987</v>
+      </c>
+      <c r="E53" s="2">
+        <v>2076.9999999999995</v>
+      </c>
+      <c r="F53" s="2">
+        <v>4676977.1911800001</v>
+      </c>
+      <c r="G53" s="2">
+        <v>30.2</v>
+      </c>
+      <c r="H53" s="2">
+        <v>300.99999999999807</v>
+      </c>
+      <c r="I53" s="2">
+        <v>303.99999999999869</v>
+      </c>
+      <c r="J53" s="2">
+        <v>783.79999999999882</v>
+      </c>
+      <c r="K53" s="2">
+        <v>202571.00000000003</v>
+      </c>
+      <c r="L53" s="2">
+        <v>87368.909999999974</v>
+      </c>
+      <c r="M53" s="2">
+        <v>8408723.8795999978</v>
+      </c>
+      <c r="N53" s="2">
+        <v>34.999999999999901</v>
+      </c>
+      <c r="O53" s="2">
+        <v>4502</v>
+      </c>
+      <c r="P53" s="2">
+        <v>19397519.885310002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>5</v>
+      </c>
+      <c r="B54" s="2">
+        <v>15028.999999999996</v>
+      </c>
+      <c r="C54" s="2">
+        <v>25869.387780000001</v>
+      </c>
+      <c r="D54" s="2">
+        <v>17235.499999999989</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1123.9999999999986</v>
+      </c>
+      <c r="F54" s="2">
+        <v>866008.93850999954</v>
+      </c>
+      <c r="G54" s="2">
+        <v>23.8</v>
+      </c>
+      <c r="H54" s="2">
+        <v>124.99999999999919</v>
+      </c>
+      <c r="I54" s="2">
+        <v>194.99999999999915</v>
+      </c>
+      <c r="J54" s="2">
+        <v>235.39999999999975</v>
+      </c>
+      <c r="K54" s="2">
+        <v>2168.999999999995</v>
+      </c>
+      <c r="L54" s="2">
+        <v>22439.059999999987</v>
+      </c>
+      <c r="M54" s="2">
+        <v>259751.15039999882</v>
+      </c>
+      <c r="N54" s="2">
+        <v>11.999999999999948</v>
+      </c>
+      <c r="O54" s="2">
+        <v>3210.9999999999995</v>
+      </c>
+      <c r="P54" s="2">
+        <v>9430951.7147999946</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>5</v>
+      </c>
+      <c r="B55" s="2">
+        <v>9192</v>
+      </c>
+      <c r="C55" s="2">
+        <v>21205.026720000002</v>
+      </c>
+      <c r="D55" s="2">
+        <v>59994</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1042.9999999999993</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1194600.3487199994</v>
+      </c>
+      <c r="G55" s="2">
+        <v>24.81</v>
+      </c>
+      <c r="H55" s="2">
+        <v>140.99999999999912</v>
+      </c>
+      <c r="I55" s="2">
+        <v>92.999999999999559</v>
+      </c>
+      <c r="J55" s="2">
+        <v>563.59999999999923</v>
+      </c>
+      <c r="K55" s="2">
+        <v>35895.999999999993</v>
+      </c>
+      <c r="L55" s="2">
+        <v>57654.419999999991</v>
+      </c>
+      <c r="M55" s="2">
+        <v>8271274.1760000018</v>
+      </c>
+      <c r="N55" s="2">
+        <v>36.999999999999908</v>
+      </c>
+      <c r="O55" s="2">
+        <v>3089.9999999999995</v>
+      </c>
+      <c r="P55" s="2">
+        <v>7029925.2345599988</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>5</v>
+      </c>
+      <c r="B56" s="2">
+        <v>11442</v>
+      </c>
+      <c r="C56" s="2">
+        <v>18218.315640000001</v>
+      </c>
+      <c r="D56" s="2">
+        <v>69421.599999999991</v>
+      </c>
+      <c r="E56" s="2">
+        <v>79.999999999999517</v>
+      </c>
+      <c r="F56" s="2">
+        <v>3389505.0556999999</v>
+      </c>
+      <c r="G56" s="2">
+        <v>21.85</v>
+      </c>
+      <c r="H56" s="2">
+        <v>164.99999999999895</v>
+      </c>
+      <c r="I56" s="2">
+        <v>248.99999999999898</v>
+      </c>
+      <c r="J56" s="2">
+        <v>369.09999999999923</v>
+      </c>
+      <c r="K56" s="2">
+        <v>18256.999999999818</v>
+      </c>
+      <c r="L56" s="2">
+        <v>57789.999999999949</v>
+      </c>
+      <c r="M56" s="2">
+        <v>521260.11459999764</v>
+      </c>
+      <c r="N56" s="2">
+        <v>5.9999999999999627</v>
+      </c>
+      <c r="O56" s="2">
+        <v>3403</v>
+      </c>
+      <c r="P56" s="2">
+        <v>5939939.1027600002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>5</v>
+      </c>
+      <c r="B57" s="2">
+        <v>2547.9999999999977</v>
+      </c>
+      <c r="C57" s="2">
+        <v>18638.87111</v>
+      </c>
+      <c r="D57" s="2">
+        <v>10254.999999999993</v>
+      </c>
+      <c r="E57" s="2">
+        <v>511.99999999999943</v>
+      </c>
+      <c r="F57" s="2">
+        <v>451466.86220999988</v>
+      </c>
+      <c r="G57" s="2">
+        <v>25</v>
+      </c>
+      <c r="H57" s="2">
+        <v>83.999999999999432</v>
+      </c>
+      <c r="I57" s="2">
+        <v>32.999999999999851</v>
+      </c>
+      <c r="J57" s="2">
+        <v>265.79999999999973</v>
+      </c>
+      <c r="K57" s="2">
+        <v>14455.999999999975</v>
+      </c>
+      <c r="L57" s="2">
+        <v>35901.049999999996</v>
+      </c>
+      <c r="M57" s="2">
+        <v>1395103.6922999984</v>
+      </c>
+      <c r="N57" s="2">
+        <v>25.999999999999936</v>
+      </c>
+      <c r="O57" s="2">
+        <v>919.99999999999955</v>
+      </c>
+      <c r="P57" s="2">
+        <v>932526.86903999816</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>5</v>
+      </c>
+      <c r="B58" s="2">
+        <v>2330.9999999999977</v>
+      </c>
+      <c r="C58" s="2">
+        <v>22823.19152</v>
+      </c>
+      <c r="D58" s="2">
+        <v>6715.4999999999927</v>
+      </c>
+      <c r="E58" s="2">
+        <v>244.99999999999955</v>
+      </c>
+      <c r="F58" s="2">
+        <v>235832.72977999973</v>
+      </c>
+      <c r="G58" s="2">
+        <v>27.3</v>
+      </c>
+      <c r="H58" s="2">
+        <v>76.99999999999946</v>
+      </c>
+      <c r="I58" s="2">
+        <v>7.9999999999999538</v>
+      </c>
+      <c r="J58" s="2">
+        <v>81.299999999999784</v>
+      </c>
+      <c r="K58" s="2">
+        <v>86576.999999999913</v>
+      </c>
+      <c r="L58" s="2">
+        <v>15944.749999999989</v>
+      </c>
+      <c r="M58" s="2">
+        <v>1820784.7858999991</v>
+      </c>
+      <c r="N58" s="2">
+        <v>15.99999999999995</v>
+      </c>
+      <c r="O58" s="2">
+        <v>729.99999999999955</v>
+      </c>
+      <c r="P58" s="2">
+        <v>1460779.4436599989</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>5</v>
+      </c>
+      <c r="B59" s="2">
+        <v>6011.9999999999982</v>
+      </c>
+      <c r="C59" s="2">
+        <v>18611.958289999999</v>
+      </c>
+      <c r="D59" s="2">
+        <v>20455.999999999993</v>
+      </c>
+      <c r="E59" s="2">
+        <v>645.99999999999943</v>
+      </c>
+      <c r="F59" s="2">
+        <v>899043.39099999995</v>
+      </c>
+      <c r="G59" s="2">
+        <v>37.19</v>
+      </c>
+      <c r="H59" s="2">
+        <v>147.99999999999906</v>
+      </c>
+      <c r="I59" s="2">
+        <v>40.999999999999794</v>
+      </c>
+      <c r="J59" s="2">
+        <v>618.49999999999932</v>
+      </c>
+      <c r="K59" s="2">
+        <v>27023.999999999942</v>
+      </c>
+      <c r="L59" s="2">
+        <v>26455.999999999993</v>
+      </c>
+      <c r="M59" s="2">
+        <v>2652645.5177999986</v>
+      </c>
+      <c r="N59" s="2">
+        <v>18.99999999999995</v>
+      </c>
+      <c r="O59" s="2">
+        <v>1149.9999999999995</v>
+      </c>
+      <c r="P59" s="2">
+        <v>6067714.9468499981</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>5</v>
+      </c>
+      <c r="B60" s="2">
+        <v>3520.9999999999991</v>
+      </c>
+      <c r="C60" s="2">
+        <v>19147.145039999999</v>
+      </c>
+      <c r="D60" s="2">
+        <v>11267.999999999993</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1097.9999999999991</v>
+      </c>
+      <c r="F60" s="2">
+        <v>584236.91447999945</v>
+      </c>
+      <c r="G60" s="2">
+        <v>51.2</v>
+      </c>
+      <c r="H60" s="2">
+        <v>122.99999999999919</v>
+      </c>
+      <c r="I60" s="2">
+        <v>36.999999999999829</v>
+      </c>
+      <c r="J60" s="2">
+        <v>408.3999999999993</v>
+      </c>
+      <c r="K60" s="2">
+        <v>38837.999999999964</v>
+      </c>
+      <c r="L60" s="2">
+        <v>26779.999999999989</v>
+      </c>
+      <c r="M60" s="2">
+        <v>2725337.6207999978</v>
+      </c>
+      <c r="N60" s="2">
+        <v>16.999999999999954</v>
+      </c>
+      <c r="O60" s="2">
+        <v>1043.9999999999995</v>
+      </c>
+      <c r="P60" s="2">
+        <v>556306.09055999748</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>5</v>
+      </c>
+      <c r="B61" s="2">
         <v>4769.9999999999982</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C61" s="2">
         <v>16996.987359999999</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D61" s="2">
         <v>11655.999999999998</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E61" s="2">
         <v>633.99999999999977</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F61" s="2">
         <v>312410.58597000001</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G61" s="2">
         <v>29.58</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H61" s="2">
         <v>71.999999999999559</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I61" s="2">
         <v>113.99999999999952</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J61" s="2">
         <v>478.49999999999966</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K61" s="2">
         <v>116217.99999999997</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L61" s="2">
         <v>29804.749999999989</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M61" s="2">
         <v>5228156.3358999994</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N61" s="2">
         <v>38.999999999999915</v>
       </c>
-      <c r="O31" s="2">
+      <c r="O61" s="2">
         <v>1186.9999999999998</v>
       </c>
-      <c r="P31" s="2">
+      <c r="P61" s="2">
         <v>2895385.0253199995</v>
       </c>
     </row>

</xml_diff>